<commit_message>
Many RubiksCube result files and small SW changes
</commit_message>
<xml_diff>
--- a/agents/RubiksCube/3x3x3_STICKER2_QT/csv/mRubiks-p13-ET16-nsym08.xlsx
+++ b/agents/RubiksCube/3x3x3_STICKER2_QT/csv/mRubiks-p13-ET16-nsym08.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wolfgang\Documents\GitHub\GBG\agents\RubiksCube\3x3x3_STICKER2_QT\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3DA109D-1F96-46C6-9C4D-6831E89479EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4883BF6-EB82-43CF-AD25-F360E01E86C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10200"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mRubiks-p13-ET16-nsym08" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -898,12 +898,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:C94"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,7 +954,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -987,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1019,7 +1018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1083,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1115,7 +1114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1147,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1179,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1211,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1243,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -1275,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1307,7 +1306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -1339,7 +1338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -1371,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -1435,7 +1434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1499,7 +1498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
@@ -1531,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -1563,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
@@ -1595,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
@@ -1627,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1691,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
@@ -1723,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0</v>
       </c>
@@ -1755,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0</v>
       </c>
@@ -1787,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -1819,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
@@ -1851,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
@@ -1915,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1947,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1979,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2043,7 +2042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2075,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2107,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1</v>
       </c>
@@ -2139,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1</v>
       </c>
@@ -2171,7 +2170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1</v>
       </c>
@@ -2203,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1</v>
       </c>
@@ -2235,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1</v>
       </c>
@@ -2267,7 +2266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1</v>
       </c>
@@ -2299,7 +2298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1</v>
       </c>
@@ -2331,7 +2330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1</v>
       </c>
@@ -2363,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1</v>
       </c>
@@ -2395,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1</v>
       </c>
@@ -2459,7 +2458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1</v>
       </c>
@@ -2491,7 +2490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1</v>
       </c>
@@ -2523,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1</v>
       </c>
@@ -2555,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1</v>
       </c>
@@ -2587,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1</v>
       </c>
@@ -2619,7 +2618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1</v>
       </c>
@@ -2651,7 +2650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1</v>
       </c>
@@ -2683,7 +2682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1</v>
       </c>
@@ -2715,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1</v>
       </c>
@@ -2747,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1</v>
       </c>
@@ -2779,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>1</v>
       </c>
@@ -2811,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1</v>
       </c>
@@ -2875,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2</v>
       </c>
@@ -2907,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2</v>
       </c>
@@ -2939,7 +2938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2</v>
       </c>
@@ -2971,7 +2970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2</v>
       </c>
@@ -3003,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2</v>
       </c>
@@ -3035,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2</v>
       </c>
@@ -3067,7 +3066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2</v>
       </c>
@@ -3099,7 +3098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2</v>
       </c>
@@ -3131,7 +3130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2</v>
       </c>
@@ -3163,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2</v>
       </c>
@@ -3195,7 +3194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2</v>
       </c>
@@ -3227,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2</v>
       </c>
@@ -3259,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2</v>
       </c>
@@ -3291,7 +3290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2</v>
       </c>
@@ -3323,7 +3322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2</v>
       </c>
@@ -3355,7 +3354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2</v>
       </c>
@@ -3387,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2</v>
       </c>
@@ -3419,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2</v>
       </c>
@@ -3451,7 +3450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2</v>
       </c>
@@ -3483,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2</v>
       </c>
@@ -3515,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2</v>
       </c>
@@ -3547,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2</v>
       </c>
@@ -3579,7 +3578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2</v>
       </c>
@@ -3611,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2</v>
       </c>
@@ -3643,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2</v>
       </c>
@@ -3675,7 +3674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2</v>
       </c>
@@ -3707,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2</v>
       </c>
@@ -3739,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2</v>
       </c>
@@ -3771,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2</v>
       </c>
@@ -3836,13 +3835,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J94">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="3000000"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A4:J94" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>